<commit_message>
Going to try move stuff to personal laptop
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kpmgaust-my.sharepoint.com/personal/jhansen3_kpmg_com_au/Documents/Documents/Python/Gambling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="11_F25DC773A252ABDACC1048C4B1DC4D7C5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF1D65AF-D5CE-4307-9182-41A8469524CE}"/>
+  <xr:revisionPtr revIDLastSave="268" documentId="11_F25DC773A252ABDACC1048C4B1DC4D7C5BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29BADFD7-A44C-4277-B6DE-D44818A8B8C7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12576" tabRatio="788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="788" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
-    <sheet name="Poker Bot" sheetId="13" r:id="rId2"/>
-    <sheet name="Basketball" sheetId="2" r:id="rId3"/>
-    <sheet name="Baseball" sheetId="3" r:id="rId4"/>
-    <sheet name="NFL" sheetId="4" r:id="rId5"/>
-    <sheet name="DFS" sheetId="5" r:id="rId6"/>
-    <sheet name="Countdown" sheetId="12" r:id="rId7"/>
-    <sheet name="Soccer" sheetId="6" r:id="rId8"/>
-    <sheet name="AFL" sheetId="9" r:id="rId9"/>
-    <sheet name="NHL" sheetId="11" r:id="rId10"/>
-    <sheet name="Quridoor" sheetId="7" r:id="rId11"/>
-    <sheet name="All Stars" sheetId="8" r:id="rId12"/>
+    <sheet name="Arbitrage" sheetId="14" r:id="rId2"/>
+    <sheet name="Poker Bot" sheetId="13" r:id="rId3"/>
+    <sheet name="Basketball" sheetId="2" r:id="rId4"/>
+    <sheet name="Baseball" sheetId="3" r:id="rId5"/>
+    <sheet name="NFL" sheetId="4" r:id="rId6"/>
+    <sheet name="DFS" sheetId="5" r:id="rId7"/>
+    <sheet name="Countdown" sheetId="12" r:id="rId8"/>
+    <sheet name="Soccer" sheetId="6" r:id="rId9"/>
+    <sheet name="AFL" sheetId="9" r:id="rId10"/>
+    <sheet name="NHL" sheetId="11" r:id="rId11"/>
+    <sheet name="Quridoor" sheetId="7" r:id="rId12"/>
+    <sheet name="All Stars" sheetId="8" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="93">
   <si>
     <t>Tidy up EVERYTHING</t>
   </si>
@@ -76,9 +77,6 @@
  - Steals</t>
   </si>
   <si>
-    <t>Update it to include more things to track like with the NFL one</t>
-  </si>
-  <si>
     <t>Fix up the folder structure</t>
   </si>
   <si>
@@ -184,12 +182,168 @@
   <si>
     <t>Need to somehow take this into consideration? Standardise it so that the percentage chance of winning and pot value equate</t>
   </si>
+  <si>
+    <t>Transition to personal laptop</t>
+  </si>
+  <si>
+    <t>Add all the other betting sites</t>
+  </si>
+  <si>
+    <t>Fix the ones that aren't working</t>
+  </si>
+  <si>
+    <t>Fix it so it pulls the correct number of games based on big win</t>
+  </si>
+  <si>
+    <t>Delete double headers?</t>
+  </si>
+  <si>
+    <t>Add other sports</t>
+  </si>
+  <si>
+    <t>Big Win Little Win?</t>
+  </si>
+  <si>
+    <t>Try catch statement for if it doesn't work the others still run</t>
+  </si>
+  <si>
+    <t>Sites</t>
+  </si>
+  <si>
+    <t>AFL</t>
+  </si>
+  <si>
+    <t>NRL</t>
+  </si>
+  <si>
+    <t>NHL</t>
+  </si>
+  <si>
+    <t>NBA</t>
+  </si>
+  <si>
+    <t>MLB</t>
+  </si>
+  <si>
+    <t>IPL</t>
+  </si>
+  <si>
+    <t>EPL</t>
+  </si>
+  <si>
+    <t>Sportsbet</t>
+  </si>
+  <si>
+    <t>Bet Deluxe</t>
+  </si>
+  <si>
+    <t>Boombet</t>
+  </si>
+  <si>
+    <t>MidasBet</t>
+  </si>
+  <si>
+    <t>Betright</t>
+  </si>
+  <si>
+    <t>Betr</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>Bet365</t>
+  </si>
+  <si>
+    <t>Ladbroked</t>
+  </si>
+  <si>
+    <t>Pointsbet</t>
+  </si>
+  <si>
+    <t>Bet Nation</t>
+  </si>
+  <si>
+    <t>Bluebet</t>
+  </si>
+  <si>
+    <t>Winnersbet</t>
+  </si>
+  <si>
+    <t>Topsport</t>
+  </si>
+  <si>
+    <t>Unibet</t>
+  </si>
+  <si>
+    <t>Dabble</t>
+  </si>
+  <si>
+    <t>Picklebet</t>
+  </si>
+  <si>
+    <t>Neds</t>
+  </si>
+  <si>
+    <t>Rob Waterhouse</t>
+  </si>
+  <si>
+    <t>Playup</t>
+  </si>
+  <si>
+    <t>Getsetbet</t>
+  </si>
+  <si>
+    <t>Collossalbet</t>
+  </si>
+  <si>
+    <t>Palmerbet</t>
+  </si>
+  <si>
+    <t>Vicbet</t>
+  </si>
+  <si>
+    <t>OkeBet</t>
+  </si>
+  <si>
+    <t>Realbookie</t>
+  </si>
+  <si>
+    <t>Save file and add to it? Or clean it and start again?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - I reckon add the date and can then filter form there</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Has the stupid draw thing so need to ignore that</t>
+  </si>
+  <si>
+    <t>No clue what isn't working</t>
+  </si>
+  <si>
+    <t>What to do when the odds aren't exact</t>
+  </si>
+  <si>
+    <t>Use Visual studio or a better IDE</t>
+  </si>
+  <si>
+    <t>What to do when there are multiple games</t>
+  </si>
+  <si>
+    <t>Conferences</t>
+  </si>
+  <si>
+    <t>Fix the match thing, need to add Draw to the list of bets</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,13 +359,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -223,10 +397,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -236,11 +411,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -516,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:B9"/>
+  <dimension ref="B2:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,12 +751,17 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -574,6 +771,31 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7C1362-4C68-496C-AF3A-B7518E3B85AF}">
+  <dimension ref="B2:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0333804-282F-4EC9-979E-04A21E6D0EA2}">
   <dimension ref="B2:B6"/>
   <sheetViews>
@@ -593,22 +815,22 @@
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -616,7 +838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B0FD3A-A8AC-4228-9FB8-F66B600AB1F9}">
   <dimension ref="B2:B3"/>
   <sheetViews>
@@ -633,7 +855,7 @@
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -641,7 +863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4DA3C1-6831-4654-A77F-A09DAAA961D4}">
   <dimension ref="B2:B8"/>
   <sheetViews>
@@ -658,32 +880,32 @@
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -692,6 +914,335 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E93B3B6-8D3D-4AAC-9B32-8CB93F71DA5C}">
+  <dimension ref="A2:I42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="5"/>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="5"/>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="5"/>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="5"/>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="5"/>
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="5"/>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="5"/>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="5"/>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
+      <c r="B42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A17:A42"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C17:I42">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA205CA2-D95E-4732-939A-ACA8B983C2AB}">
   <dimension ref="B2:C10"/>
   <sheetViews>
@@ -706,47 +1257,47 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -755,7 +1306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D082729-AE8F-48FC-BC06-E02063E1B62B}">
   <dimension ref="B2:B4"/>
   <sheetViews>
@@ -780,7 +1331,7 @@
     </row>
     <row r="4" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -789,12 +1340,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3D1033-2FF2-4473-ACAA-F1675DA18EE7}">
-  <dimension ref="B2:B3"/>
+  <dimension ref="B2:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,7 +1357,12 @@
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -814,7 +1370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9725C570-AE60-4AC5-9671-3F2ACA611167}">
   <dimension ref="B2:B4"/>
   <sheetViews>
@@ -844,7 +1400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4561525-3D34-41C7-BE0C-65B4F08B7ACD}">
   <dimension ref="B2:B8"/>
   <sheetViews>
@@ -864,27 +1420,27 @@
     </row>
     <row r="3" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -892,7 +1448,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCC5232-E38D-4A98-A17D-2BCC747EA02F}">
   <dimension ref="B2:B6"/>
   <sheetViews>
@@ -909,22 +1465,22 @@
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -933,7 +1489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC696E5-BFF1-4845-B891-F5CBE0588BFC}">
   <dimension ref="B2:B3"/>
   <sheetViews>
@@ -950,32 +1506,7 @@
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7C1362-4C68-496C-AF3A-B7518E3B85AF}">
-  <dimension ref="B2:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>